<commit_message>
Used a data table for one solution
</commit_message>
<xml_diff>
--- a/CH-047 Multiple text replaces.xlsx
+++ b/CH-047 Multiple text replaces.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC332C84-3059-4A50-A385-FC7AC5CD6D75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A182396-F26C-4C33-A5F5-B05FC7831432}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="38">
   <si>
     <t>Result</t>
   </si>
@@ -167,6 +167,12 @@
   </si>
   <si>
     <t>New</t>
+  </si>
+  <si>
+    <t>SCAN grabs just one item at a time.</t>
+  </si>
+  <si>
+    <t>Can't find a way to use byrow</t>
   </si>
 </sst>
 </file>
@@ -222,7 +228,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -247,6 +253,30 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="14">
     <border>
@@ -443,7 +473,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -517,6 +547,20 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="2" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1658,10 +1702,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7D7FD7E-DCE8-44B1-9D22-42CE74375CB6}">
-  <dimension ref="B1:M28"/>
+  <dimension ref="B1:Q28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+      <selection activeCell="S23" sqref="S23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1674,9 +1718,12 @@
     <col min="7" max="9" width="9.19921875" style="1" customWidth="1"/>
     <col min="10" max="10" width="12.59765625" style="1" customWidth="1"/>
     <col min="12" max="12" width="9.3984375" customWidth="1"/>
+    <col min="14" max="14" width="13.8984375" customWidth="1"/>
+    <col min="15" max="15" width="10.69921875" customWidth="1"/>
+    <col min="16" max="16" width="11.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B1" s="13" t="s">
         <v>1</v>
       </c>
@@ -1693,7 +1740,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="2:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:17" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="15" t="s">
         <v>2</v>
       </c>
@@ -1711,8 +1758,19 @@
       <c r="J2" s="20" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="2:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M2" s="30" t="str">
+        <f>B3</f>
+        <v>X-MN12 21</v>
+      </c>
+      <c r="N2" s="31" t="str" cm="1">
+        <f t="array" ref="N2">_xlfn.REDUCE(M2,_xlfn.SEQUENCE(ROWS(E3:E10)),_xlfn.LAMBDA(_xlpm.a,_xlpm.v,SUBSTITUTE(_xlpm.a,INDEX(E3:E10,_xlpm.v),INDEX(F3:F10,_xlpm.v))))</f>
+        <v>P1MN12-21</v>
+      </c>
+      <c r="O2" s="27"/>
+      <c r="P2" s="27"/>
+      <c r="Q2" s="27"/>
+    </row>
+    <row r="3" spans="2:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B3" s="12" t="s">
         <v>3</v>
       </c>
@@ -1730,8 +1788,13 @@
       <c r="J3" s="21" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="4" spans="2:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M3" s="28"/>
+      <c r="N3" s="28"/>
+      <c r="O3" s="28"/>
+      <c r="P3" s="28"/>
+      <c r="Q3" s="28"/>
+    </row>
+    <row r="4" spans="2:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="12" t="s">
         <v>4</v>
       </c>
@@ -1749,8 +1812,16 @@
       <c r="J4" s="21" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="5" spans="2:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M4" s="28"/>
+      <c r="N4" s="28"/>
+      <c r="O4" s="28"/>
+      <c r="P4" s="32" t="str">
+        <f>N2</f>
+        <v>P1MN12-21</v>
+      </c>
+      <c r="Q4" s="28"/>
+    </row>
+    <row r="5" spans="2:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B5" s="12" t="s">
         <v>5</v>
       </c>
@@ -1768,8 +1839,21 @@
       <c r="J5" s="21" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="6" spans="2:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M5" s="28"/>
+      <c r="N5" s="28"/>
+      <c r="O5" s="28" t="s">
+        <v>3</v>
+      </c>
+      <c r="P5" s="28" t="str">
+        <f t="dataTable" ref="P5:P13" dt2D="0" dtr="0" r1="M2"/>
+        <v>P1MN12-21</v>
+      </c>
+      <c r="Q5" s="33" t="b" cm="1">
+        <f t="array" ref="Q5:Q13">J3:J11=P5:P13</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="2:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="12" t="s">
         <v>6</v>
       </c>
@@ -1787,8 +1871,19 @@
       <c r="J6" s="21" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="7" spans="2:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M6" s="28"/>
+      <c r="N6" s="28"/>
+      <c r="O6" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="P6" s="28" t="str">
+        <v>P1MN11-13</v>
+      </c>
+      <c r="Q6" s="33" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="2:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="12" t="s">
         <v>7</v>
       </c>
@@ -1806,8 +1901,19 @@
       <c r="J7" s="21" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="8" spans="2:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M7" s="28"/>
+      <c r="N7" s="28"/>
+      <c r="O7" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="P7" s="28" t="str">
+        <v>P2MM14-15</v>
+      </c>
+      <c r="Q7" s="33" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="2:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B8" s="12" t="s">
         <v>8</v>
       </c>
@@ -1825,8 +1931,19 @@
       <c r="J8" s="21" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="9" spans="2:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M8" s="28"/>
+      <c r="N8" s="28"/>
+      <c r="O8" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="P8" s="28" t="str">
+        <v>P2AC14-21</v>
+      </c>
+      <c r="Q8" s="33" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="2:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B9" s="12" t="s">
         <v>9</v>
       </c>
@@ -1844,8 +1961,19 @@
       <c r="J9" s="21" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="10" spans="2:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M9" s="28"/>
+      <c r="N9" s="28"/>
+      <c r="O9" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="P9" s="28" t="str">
+        <v>P1MC06-11</v>
+      </c>
+      <c r="Q9" s="33" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="2:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B10" s="12" t="s">
         <v>10</v>
       </c>
@@ -1863,8 +1991,19 @@
       <c r="J10" s="21" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="11" spans="2:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M10" s="28"/>
+      <c r="N10" s="28"/>
+      <c r="O10" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="P10" s="28" t="str">
+        <v>P1AN21-25</v>
+      </c>
+      <c r="Q10" s="33" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="2:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B11" s="23" t="s">
         <v>11</v>
       </c>
@@ -1879,9 +2018,19 @@
         <v>32</v>
       </c>
       <c r="L11"/>
-      <c r="M11"/>
-    </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="M11" s="29"/>
+      <c r="N11" s="28"/>
+      <c r="O11" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="P11" s="28" t="str">
+        <v>P1AQ21-21</v>
+      </c>
+      <c r="Q11" s="33" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
       <c r="E12" s="7"/>
@@ -1889,8 +2038,19 @@
       <c r="G12" s="7"/>
       <c r="H12" s="7"/>
       <c r="I12" s="7"/>
-    </row>
-    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="M12" s="29"/>
+      <c r="N12" s="29"/>
+      <c r="O12" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="P12" s="29" t="str">
+        <v>P1SS50-02</v>
+      </c>
+      <c r="Q12" s="34" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C13" s="7"/>
       <c r="D13" s="7"/>
       <c r="E13" s="7"/>
@@ -1898,8 +2058,19 @@
       <c r="G13" s="7"/>
       <c r="H13" s="7"/>
       <c r="I13" s="7"/>
-    </row>
-    <row r="14" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="M13" s="29"/>
+      <c r="N13" s="29"/>
+      <c r="O13" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="P13" s="29" t="str">
+        <v>P3FJ10-12</v>
+      </c>
+      <c r="Q13" s="34" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C14" s="7"/>
       <c r="D14" s="7"/>
       <c r="E14" s="7"/>
@@ -1908,7 +2079,7 @@
       <c r="H14" s="7"/>
       <c r="I14" s="7"/>
     </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C15" s="7"/>
       <c r="D15" s="7"/>
       <c r="E15" s="7"/>
@@ -1917,7 +2088,7 @@
       <c r="H15" s="7"/>
       <c r="I15" s="7"/>
     </row>
-    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C16" s="7"/>
       <c r="D16" s="7"/>
       <c r="E16" s="7"/>
@@ -1925,8 +2096,11 @@
       <c r="G16" s="7"/>
       <c r="H16" s="7"/>
       <c r="I16" s="7"/>
-    </row>
-    <row r="17" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="N16" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C17" s="7"/>
       <c r="D17" s="7"/>
       <c r="E17" s="7"/>
@@ -1935,7 +2109,7 @@
       <c r="H17" s="7"/>
       <c r="I17" s="7"/>
     </row>
-    <row r="18" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C18" s="7"/>
       <c r="D18" s="7"/>
       <c r="E18" s="7"/>
@@ -1953,13 +2127,30 @@
       <c r="G18" s="7"/>
       <c r="H18" s="7"/>
       <c r="I18" s="7"/>
-    </row>
-    <row r="19" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="J18" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="N18" t="str" cm="1">
+        <f t="array" ref="N18:N25">_xlfn.BYROW(E3:F10,_xlfn.LAMBDA(_xlpm.r,SUBSTITUTE(B3,_xlfn.TAKE(_xlpm.r,1,1),_xlfn.TAKE(_xlpm.r,1,-1))))</f>
+        <v>P1MN12 21</v>
+      </c>
+    </row>
+    <row r="19" spans="3:14" x14ac:dyDescent="0.25">
       <c r="F19" s="20" t="str">
         <v>Product IDs</v>
       </c>
-    </row>
-    <row r="20" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="J19" s="1" cm="1">
+        <f t="array" ref="J19:K26">_xlfn.SCAN(B3,E3:F10,_xlfn.LAMBDA(_xlpm.a,_xlpm.v,LEN(_xlpm.v)))</f>
+        <v>2</v>
+      </c>
+      <c r="K19">
+        <v>2</v>
+      </c>
+      <c r="N19" t="str">
+        <v>X-MN12 21</v>
+      </c>
+    </row>
+    <row r="20" spans="3:14" x14ac:dyDescent="0.25">
       <c r="F20" s="21" t="str">
         <v>P1MN12-21</v>
       </c>
@@ -1967,56 +2158,116 @@
         <f t="array" ref="H20:H28">F20:F28=J3:J11</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="J20" s="1">
+        <v>2</v>
+      </c>
+      <c r="K20">
+        <v>2</v>
+      </c>
+      <c r="N20" t="str">
+        <v>X-MN12 21</v>
+      </c>
+    </row>
+    <row r="21" spans="3:14" x14ac:dyDescent="0.25">
       <c r="F21" s="21" t="str">
         <v>P1MN11-13</v>
       </c>
       <c r="H21" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="J21" s="1">
+        <v>2</v>
+      </c>
+      <c r="K21">
+        <v>2</v>
+      </c>
+      <c r="N21" t="str">
+        <v>X-MN12-21</v>
+      </c>
+    </row>
+    <row r="22" spans="3:14" x14ac:dyDescent="0.25">
       <c r="F22" s="21" t="str">
         <v>P2MM14-15</v>
       </c>
       <c r="H22" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="J22" s="1">
+        <v>1</v>
+      </c>
+      <c r="K22">
+        <v>1</v>
+      </c>
+      <c r="N22" t="str">
+        <v>X-MN12 21</v>
+      </c>
+    </row>
+    <row r="23" spans="3:14" x14ac:dyDescent="0.25">
       <c r="F23" s="21" t="str">
         <v>P2AC14-21</v>
       </c>
       <c r="H23" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="J23" s="1">
+        <v>1</v>
+      </c>
+      <c r="K23">
+        <v>1</v>
+      </c>
+      <c r="N23" t="str">
+        <v>X-MN12 21</v>
+      </c>
+    </row>
+    <row r="24" spans="3:14" x14ac:dyDescent="0.25">
       <c r="F24" s="21" t="str">
         <v>P1MC06-11</v>
       </c>
       <c r="H24" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="J24" s="1">
+        <v>1</v>
+      </c>
+      <c r="K24">
+        <v>1</v>
+      </c>
+      <c r="N24" t="str">
+        <v>X-MN12 21</v>
+      </c>
+    </row>
+    <row r="25" spans="3:14" x14ac:dyDescent="0.25">
       <c r="F25" s="21" t="str">
         <v>P1AN21-25</v>
       </c>
       <c r="H25" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="J25" s="1">
+        <v>1</v>
+      </c>
+      <c r="K25">
+        <v>1</v>
+      </c>
+      <c r="N25" t="str">
+        <v>X-MN12 21</v>
+      </c>
+    </row>
+    <row r="26" spans="3:14" x14ac:dyDescent="0.25">
       <c r="F26" s="21" t="str">
         <v>P1AQ21-21</v>
       </c>
       <c r="H26" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="J26" s="1">
+        <v>1</v>
+      </c>
+      <c r="K26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="3:14" x14ac:dyDescent="0.25">
       <c r="F27" s="21" t="str">
         <v>P1SS50-02</v>
       </c>
@@ -2024,7 +2275,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:14" x14ac:dyDescent="0.25">
       <c r="F28" s="22" t="str">
         <v>P3FJ10-12</v>
       </c>

</xml_diff>

<commit_message>
Mentioned my approach to data tables
</commit_message>
<xml_diff>
--- a/CH-047 Multiple text replaces.xlsx
+++ b/CH-047 Multiple text replaces.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A182396-F26C-4C33-A5F5-B05FC7831432}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8396C3BE-F91F-44FD-B6B0-27BD27667A94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="39">
   <si>
     <t>Result</t>
   </si>
@@ -173,6 +173,9 @@
   </si>
   <si>
     <t>Can't find a way to use byrow</t>
+  </si>
+  <si>
+    <t>I still like the use of data tables for experiments</t>
   </si>
 </sst>
 </file>
@@ -541,12 +544,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -561,6 +558,12 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1424,10 +1427,10 @@
       </c>
       <c r="C1" s="6"/>
       <c r="D1" s="6"/>
-      <c r="E1" s="25" t="s">
+      <c r="E1" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="F1" s="26"/>
+      <c r="F1" s="34"/>
       <c r="G1" s="6"/>
       <c r="H1" s="6"/>
       <c r="I1" s="6"/>
@@ -1705,7 +1708,7 @@
   <dimension ref="B1:Q28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S23" sqref="S23"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1729,18 +1732,21 @@
       </c>
       <c r="C1" s="6"/>
       <c r="D1" s="6"/>
-      <c r="E1" s="25" t="s">
+      <c r="E1" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="F1" s="26"/>
+      <c r="F1" s="34"/>
       <c r="G1" s="6"/>
       <c r="H1" s="6"/>
       <c r="I1" s="6"/>
       <c r="J1" s="14" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="2:17" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M1" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="2:17" s="5" customFormat="1" ht="27.6" x14ac:dyDescent="0.25">
       <c r="B2" s="15" t="s">
         <v>2</v>
       </c>
@@ -1758,17 +1764,17 @@
       <c r="J2" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="M2" s="30" t="str">
+      <c r="M2" s="28" t="str">
         <f>B3</f>
         <v>X-MN12 21</v>
       </c>
-      <c r="N2" s="31" t="str" cm="1">
+      <c r="N2" s="29" t="str" cm="1">
         <f t="array" ref="N2">_xlfn.REDUCE(M2,_xlfn.SEQUENCE(ROWS(E3:E10)),_xlfn.LAMBDA(_xlpm.a,_xlpm.v,SUBSTITUTE(_xlpm.a,INDEX(E3:E10,_xlpm.v),INDEX(F3:F10,_xlpm.v))))</f>
         <v>P1MN12-21</v>
       </c>
-      <c r="O2" s="27"/>
-      <c r="P2" s="27"/>
-      <c r="Q2" s="27"/>
+      <c r="O2" s="25"/>
+      <c r="P2" s="25"/>
+      <c r="Q2" s="25"/>
     </row>
     <row r="3" spans="2:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B3" s="12" t="s">
@@ -1788,11 +1794,11 @@
       <c r="J3" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="M3" s="28"/>
-      <c r="N3" s="28"/>
-      <c r="O3" s="28"/>
-      <c r="P3" s="28"/>
-      <c r="Q3" s="28"/>
+      <c r="M3" s="26"/>
+      <c r="N3" s="26"/>
+      <c r="O3" s="26"/>
+      <c r="P3" s="26"/>
+      <c r="Q3" s="26"/>
     </row>
     <row r="4" spans="2:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="12" t="s">
@@ -1812,14 +1818,14 @@
       <c r="J4" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="M4" s="28"/>
-      <c r="N4" s="28"/>
-      <c r="O4" s="28"/>
-      <c r="P4" s="32" t="str">
+      <c r="M4" s="26"/>
+      <c r="N4" s="26"/>
+      <c r="O4" s="26"/>
+      <c r="P4" s="30" t="str">
         <f>N2</f>
         <v>P1MN12-21</v>
       </c>
-      <c r="Q4" s="28"/>
+      <c r="Q4" s="26"/>
     </row>
     <row r="5" spans="2:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B5" s="12" t="s">
@@ -1839,16 +1845,16 @@
       <c r="J5" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="M5" s="28"/>
-      <c r="N5" s="28"/>
-      <c r="O5" s="28" t="s">
+      <c r="M5" s="26"/>
+      <c r="N5" s="26"/>
+      <c r="O5" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="P5" s="28" t="str">
+      <c r="P5" s="26" t="str">
         <f t="dataTable" ref="P5:P13" dt2D="0" dtr="0" r1="M2"/>
         <v>P1MN12-21</v>
       </c>
-      <c r="Q5" s="33" t="b" cm="1">
+      <c r="Q5" s="31" t="b" cm="1">
         <f t="array" ref="Q5:Q13">J3:J11=P5:P13</f>
         <v>1</v>
       </c>
@@ -1871,15 +1877,15 @@
       <c r="J6" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="M6" s="28"/>
-      <c r="N6" s="28"/>
-      <c r="O6" s="28" t="s">
+      <c r="M6" s="26"/>
+      <c r="N6" s="26"/>
+      <c r="O6" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="P6" s="28" t="str">
+      <c r="P6" s="26" t="str">
         <v>P1MN11-13</v>
       </c>
-      <c r="Q6" s="33" t="b">
+      <c r="Q6" s="31" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1901,15 +1907,15 @@
       <c r="J7" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="M7" s="28"/>
-      <c r="N7" s="28"/>
-      <c r="O7" s="28" t="s">
+      <c r="M7" s="26"/>
+      <c r="N7" s="26"/>
+      <c r="O7" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="P7" s="28" t="str">
+      <c r="P7" s="26" t="str">
         <v>P2MM14-15</v>
       </c>
-      <c r="Q7" s="33" t="b">
+      <c r="Q7" s="31" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1931,15 +1937,15 @@
       <c r="J8" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="M8" s="28"/>
-      <c r="N8" s="28"/>
-      <c r="O8" s="28" t="s">
+      <c r="M8" s="26"/>
+      <c r="N8" s="26"/>
+      <c r="O8" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="P8" s="28" t="str">
+      <c r="P8" s="26" t="str">
         <v>P2AC14-21</v>
       </c>
-      <c r="Q8" s="33" t="b">
+      <c r="Q8" s="31" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1961,15 +1967,15 @@
       <c r="J9" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="M9" s="28"/>
-      <c r="N9" s="28"/>
-      <c r="O9" s="28" t="s">
+      <c r="M9" s="26"/>
+      <c r="N9" s="26"/>
+      <c r="O9" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="P9" s="28" t="str">
+      <c r="P9" s="26" t="str">
         <v>P1MC06-11</v>
       </c>
-      <c r="Q9" s="33" t="b">
+      <c r="Q9" s="31" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1991,15 +1997,15 @@
       <c r="J10" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="M10" s="28"/>
-      <c r="N10" s="28"/>
-      <c r="O10" s="28" t="s">
+      <c r="M10" s="26"/>
+      <c r="N10" s="26"/>
+      <c r="O10" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="P10" s="28" t="str">
+      <c r="P10" s="26" t="str">
         <v>P1AN21-25</v>
       </c>
-      <c r="Q10" s="33" t="b">
+      <c r="Q10" s="31" t="b">
         <v>1</v>
       </c>
     </row>
@@ -2018,15 +2024,15 @@
         <v>32</v>
       </c>
       <c r="L11"/>
-      <c r="M11" s="29"/>
-      <c r="N11" s="28"/>
-      <c r="O11" s="28" t="s">
+      <c r="M11" s="27"/>
+      <c r="N11" s="26"/>
+      <c r="O11" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="P11" s="28" t="str">
+      <c r="P11" s="26" t="str">
         <v>P1AQ21-21</v>
       </c>
-      <c r="Q11" s="33" t="b">
+      <c r="Q11" s="31" t="b">
         <v>1</v>
       </c>
     </row>
@@ -2038,15 +2044,15 @@
       <c r="G12" s="7"/>
       <c r="H12" s="7"/>
       <c r="I12" s="7"/>
-      <c r="M12" s="29"/>
-      <c r="N12" s="29"/>
-      <c r="O12" s="29" t="s">
+      <c r="M12" s="27"/>
+      <c r="N12" s="27"/>
+      <c r="O12" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="P12" s="29" t="str">
+      <c r="P12" s="27" t="str">
         <v>P1SS50-02</v>
       </c>
-      <c r="Q12" s="34" t="b">
+      <c r="Q12" s="32" t="b">
         <v>1</v>
       </c>
     </row>
@@ -2058,15 +2064,15 @@
       <c r="G13" s="7"/>
       <c r="H13" s="7"/>
       <c r="I13" s="7"/>
-      <c r="M13" s="29"/>
-      <c r="N13" s="29"/>
-      <c r="O13" s="29" t="s">
+      <c r="M13" s="27"/>
+      <c r="N13" s="27"/>
+      <c r="O13" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="P13" s="29" t="str">
+      <c r="P13" s="27" t="str">
         <v>P3FJ10-12</v>
       </c>
-      <c r="Q13" s="34" t="b">
+      <c r="Q13" s="32" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>